<commit_message>
Updated DEU model - 2025-08-31 18:43
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_DEU/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7421B60-CF12-44EC-838B-D18A058E1D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A26BEA5-B439-4069-8796-A0E85032A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E6F4BF-048B-B331-F565-91745DE7B37A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F90DBE-8B44-B649-DA1D-A8291759CDC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>

<commit_message>
Updated DEU model - 2025-09-01 00:49
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_DEU/SuppXLS/Scen_Base_VS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C91FBC5E-2711-4B14-8047-2B96FC96DA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D0864BC-B4BF-44B3-9AD7-D459D57CB467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="92">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>~UC_T: uc_rhsrt</t>
+  </si>
+  <si>
+    <t>\I: solar</t>
+  </si>
+  <si>
+    <t>\I: wind</t>
   </si>
   <si>
     <t>geothermal</t>
@@ -624,7 +630,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DE788F5-F243-64A4-0A83-2F5F654C9C92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2672FAA6-9FC5-A098-D934-918F57F090F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -978,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1116,17 +1122,17 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="4" t="str">
         <f>IFERROR(MIN(VLOOKUP(B6,$F$3:$J$11,5,FALSE),$A$6),"")</f>
-        <v>0.11452491530550409</v>
+        <v/>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1145,7 +1151,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1383,7 +1389,7 @@
     </row>
     <row r="11" spans="1:38" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1396,7 +1402,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.45">
       <c r="F12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G12" s="3">
         <v>0.13646444879321595</v>
@@ -1730,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320A1887-1B0C-44A8-9658-90FD86FEE0A5}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1745,7 +1751,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1757,12 +1763,12 @@
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>70</v>
@@ -1791,7 +1797,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C11" s="19">
         <v>10</v>
@@ -2124,7 +2130,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B11" s="12">
         <v>2000</v>
@@ -2250,7 +2256,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B20" s="14">
         <v>2001</v>
@@ -2376,7 +2382,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B29" s="12">
         <v>2002</v>
@@ -2502,7 +2508,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B38" s="14">
         <v>2003</v>
@@ -2628,7 +2634,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B47" s="12">
         <v>2004</v>
@@ -2754,7 +2760,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B56" s="14">
         <v>2005</v>
@@ -2880,7 +2886,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B65" s="12">
         <v>2006</v>
@@ -3006,7 +3012,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B74" s="14">
         <v>2007</v>
@@ -3132,7 +3138,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B83" s="12">
         <v>2008</v>
@@ -3258,7 +3264,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B92" s="14">
         <v>2009</v>
@@ -3384,7 +3390,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B101" s="12">
         <v>2010</v>
@@ -3510,7 +3516,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B110" s="14">
         <v>2011</v>
@@ -3636,7 +3642,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B119" s="12">
         <v>2012</v>
@@ -3762,7 +3768,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B128" s="14">
         <v>2013</v>
@@ -3888,7 +3894,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B137" s="12">
         <v>2014</v>
@@ -4014,7 +4020,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B146" s="14">
         <v>2015</v>
@@ -4140,7 +4146,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B155" s="12">
         <v>2016</v>
@@ -4266,7 +4272,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B164" s="14">
         <v>2017</v>
@@ -4392,7 +4398,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B173" s="12">
         <v>2018</v>
@@ -4518,7 +4524,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B182" s="14">
         <v>2019</v>
@@ -4644,7 +4650,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A191" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B191" s="12">
         <v>2020</v>
@@ -4770,7 +4776,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B200" s="14">
         <v>2021</v>
@@ -4896,7 +4902,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A209" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B209" s="12">
         <v>2022</v>
@@ -5022,7 +5028,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A218" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B218" s="14">
         <v>2023</v>
@@ -5148,7 +5154,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A227" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B227" s="12">
         <v>2000</v>
@@ -5274,7 +5280,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A236" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B236" s="14">
         <v>2001</v>
@@ -5400,7 +5406,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A245" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B245" s="12">
         <v>2002</v>
@@ -5526,7 +5532,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A254" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B254" s="14">
         <v>2003</v>
@@ -5652,7 +5658,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A263" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B263" s="12">
         <v>2004</v>
@@ -5778,7 +5784,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A272" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B272" s="14">
         <v>2005</v>
@@ -5904,7 +5910,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A281" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B281" s="12">
         <v>2006</v>
@@ -6030,7 +6036,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A290" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B290" s="14">
         <v>2007</v>
@@ -6156,7 +6162,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A299" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B299" s="12">
         <v>2008</v>
@@ -6282,7 +6288,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A308" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B308" s="14">
         <v>2009</v>
@@ -6408,7 +6414,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A317" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B317" s="12">
         <v>2010</v>
@@ -6534,7 +6540,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A326" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B326" s="14">
         <v>2011</v>
@@ -6660,7 +6666,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A335" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B335" s="12">
         <v>2012</v>
@@ -6786,7 +6792,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A344" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B344" s="14">
         <v>2013</v>
@@ -6912,7 +6918,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A353" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B353" s="12">
         <v>2014</v>
@@ -7038,7 +7044,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A362" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B362" s="14">
         <v>2015</v>
@@ -7164,7 +7170,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A371" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B371" s="12">
         <v>2016</v>
@@ -7290,7 +7296,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A380" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B380" s="14">
         <v>2017</v>
@@ -7416,7 +7422,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A389" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B389" s="12">
         <v>2018</v>
@@ -7542,7 +7548,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A398" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B398" s="14">
         <v>2019</v>
@@ -7668,7 +7674,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A407" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B407" s="12">
         <v>2020</v>
@@ -7794,7 +7800,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A416" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B416" s="14">
         <v>2021</v>
@@ -7920,7 +7926,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A425" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B425" s="12">
         <v>2022</v>
@@ -8046,7 +8052,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A434" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B434" s="14">
         <v>2023</v>
@@ -8172,7 +8178,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A443" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B443" s="12">
         <v>2000</v>
@@ -8298,7 +8304,7 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A452" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B452" s="14">
         <v>2001</v>
@@ -8424,7 +8430,7 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A461" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B461" s="12">
         <v>2002</v>
@@ -8550,7 +8556,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A470" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B470" s="14">
         <v>2003</v>
@@ -8676,7 +8682,7 @@
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A479" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B479" s="12">
         <v>2004</v>
@@ -8802,7 +8808,7 @@
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A488" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B488" s="14">
         <v>2005</v>
@@ -8928,7 +8934,7 @@
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A497" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B497" s="12">
         <v>2006</v>
@@ -9054,7 +9060,7 @@
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A506" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B506" s="14">
         <v>2007</v>
@@ -9180,7 +9186,7 @@
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A515" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B515" s="12">
         <v>2008</v>
@@ -9306,7 +9312,7 @@
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A524" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B524" s="14">
         <v>2009</v>
@@ -9432,7 +9438,7 @@
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A533" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B533" s="12">
         <v>2010</v>
@@ -9558,7 +9564,7 @@
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A542" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B542" s="14">
         <v>2011</v>
@@ -9684,7 +9690,7 @@
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A551" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B551" s="12">
         <v>2012</v>
@@ -9810,7 +9816,7 @@
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A560" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B560" s="14">
         <v>2013</v>
@@ -9936,7 +9942,7 @@
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A569" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B569" s="12">
         <v>2014</v>
@@ -10062,7 +10068,7 @@
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A578" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B578" s="14">
         <v>2015</v>
@@ -10188,7 +10194,7 @@
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A587" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B587" s="12">
         <v>2016</v>
@@ -10314,7 +10320,7 @@
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A596" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B596" s="14">
         <v>2017</v>
@@ -10440,7 +10446,7 @@
     </row>
     <row r="605" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A605" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B605" s="12">
         <v>2018</v>
@@ -10566,7 +10572,7 @@
     </row>
     <row r="614" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A614" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B614" s="14">
         <v>2019</v>
@@ -10692,7 +10698,7 @@
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A623" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B623" s="12">
         <v>2020</v>
@@ -10818,7 +10824,7 @@
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A632" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B632" s="14">
         <v>2021</v>
@@ -10944,7 +10950,7 @@
     </row>
     <row r="641" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A641" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B641" s="12">
         <v>2022</v>
@@ -11070,7 +11076,7 @@
     </row>
     <row r="650" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A650" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B650" s="14">
         <v>2023</v>

</xml_diff>